<commit_message>
added secret agents for bad man
</commit_message>
<xml_diff>
--- a/reports/ProjectPlan.xlsx
+++ b/reports/ProjectPlan.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="69">
   <si>
     <t>Project Planner</t>
   </si>
@@ -718,137 +718,137 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="8" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="8">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="12" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="10" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="10" applyNumberFormat="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="10" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="10" applyNumberFormat="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="8" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="8">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="12" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1723,7 +1723,7 @@
   <dimension ref="B1:HH35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:I3"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1732,7 +1732,7 @@
     <col min="2" max="2" width="13" style="2" customWidth="1"/>
     <col min="3" max="3" width="13.875" style="2" customWidth="1"/>
     <col min="4" max="4" width="70.625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12" style="51" customWidth="1"/>
+    <col min="5" max="5" width="12" style="31" customWidth="1"/>
     <col min="6" max="6" width="11.625" style="16" customWidth="1"/>
     <col min="7" max="7" width="11.625" style="1" customWidth="1"/>
     <col min="8" max="8" width="11.625" style="16" customWidth="1"/>
@@ -1743,85 +1743,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:216" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="52"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="32"/>
     </row>
     <row r="2" spans="2:216" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="47" t="s">
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="48" t="s">
+      <c r="G2" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="49" t="s">
+      <c r="H2" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="50" t="s">
+      <c r="I2" s="30" t="s">
         <v>57</v>
       </c>
       <c r="J2" s="7"/>
     </row>
     <row r="3" spans="2:216" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="54" t="s">
+      <c r="B3" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
       <c r="J3"/>
       <c r="K3" s="8"/>
-      <c r="L3" s="26" t="s">
+      <c r="L3" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="27"/>
-      <c r="N3" s="27"/>
-      <c r="O3" s="27"/>
-      <c r="P3" s="28"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="53"/>
+      <c r="O3" s="53"/>
+      <c r="P3" s="54"/>
       <c r="Q3" s="9"/>
-      <c r="R3" s="26" t="s">
+      <c r="R3" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="29"/>
-      <c r="T3" s="29"/>
-      <c r="U3" s="28"/>
+      <c r="S3" s="55"/>
+      <c r="T3" s="55"/>
+      <c r="U3" s="54"/>
       <c r="V3" s="10"/>
-      <c r="W3" s="17" t="s">
+      <c r="W3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="X3" s="18"/>
-      <c r="Y3" s="18"/>
-      <c r="Z3" s="30"/>
+      <c r="X3" s="57"/>
+      <c r="Y3" s="57"/>
+      <c r="Z3" s="58"/>
       <c r="AA3" s="11"/>
-      <c r="AB3" s="31" t="s">
+      <c r="AB3" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" s="32"/>
-      <c r="AD3" s="32"/>
-      <c r="AE3" s="32"/>
-      <c r="AF3" s="56"/>
+      <c r="AC3" s="42"/>
+      <c r="AD3" s="42"/>
+      <c r="AE3" s="42"/>
+      <c r="AF3" s="34"/>
       <c r="AG3" s="12"/>
-      <c r="AH3" s="31" t="s">
+      <c r="AH3" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="AI3" s="32"/>
-      <c r="AJ3" s="32"/>
-      <c r="AK3" s="32"/>
-      <c r="AL3" s="32"/>
-      <c r="AO3" s="56"/>
-      <c r="AP3" s="56"/>
-      <c r="AQ3" s="56"/>
+      <c r="AI3" s="42"/>
+      <c r="AJ3" s="42"/>
+      <c r="AK3" s="42"/>
+      <c r="AL3" s="42"/>
+      <c r="AO3" s="34"/>
+      <c r="AP3" s="34"/>
+      <c r="AQ3" s="34"/>
       <c r="AR3"/>
       <c r="AS3"/>
       <c r="AT3"/>
@@ -1831,31 +1831,31 @@
       <c r="AX3"/>
     </row>
     <row r="4" spans="2:216" s="6" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="23" t="s">
+      <c r="I4" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="50" t="s">
         <v>9</v>
       </c>
       <c r="K4" s="13" t="s">
@@ -1921,15 +1921,15 @@
       <c r="BQ4" s="5"/>
     </row>
     <row r="5" spans="2:216" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="20"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="58"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="51"/>
       <c r="K5" s="14">
         <v>42991</v>
       </c>
@@ -2550,750 +2550,798 @@
       </c>
     </row>
     <row r="6" spans="2:216" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="E6" s="59" t="s">
+      <c r="E6" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="39">
+      <c r="F6" s="19">
         <v>42991</v>
       </c>
-      <c r="G6" s="40">
+      <c r="G6" s="20">
         <v>14</v>
       </c>
-      <c r="H6" s="41">
+      <c r="H6" s="21">
         <v>42991</v>
       </c>
-      <c r="I6" s="40">
+      <c r="I6" s="20">
         <v>22</v>
       </c>
-      <c r="J6" s="42">
+      <c r="J6" s="22">
         <v>1</v>
       </c>
-      <c r="K6" s="55"/>
+      <c r="K6" s="33"/>
     </row>
     <row r="7" spans="2:216" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="38" t="s">
+      <c r="D7" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="59" t="s">
+      <c r="E7" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="F7" s="39">
+      <c r="F7" s="19">
         <v>43013</v>
       </c>
-      <c r="G7" s="40">
+      <c r="G7" s="20">
         <v>7</v>
       </c>
-      <c r="H7" s="39">
+      <c r="H7" s="19">
         <v>43027</v>
       </c>
-      <c r="I7" s="40">
+      <c r="I7" s="20">
         <v>1</v>
       </c>
-      <c r="J7" s="42">
+      <c r="J7" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:216" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="E8" s="59" t="s">
+      <c r="E8" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="F8" s="39">
+      <c r="F8" s="19">
         <v>43027</v>
       </c>
-      <c r="G8" s="40">
+      <c r="G8" s="20">
         <v>1</v>
       </c>
-      <c r="H8" s="39">
+      <c r="H8" s="19">
         <v>43027</v>
       </c>
-      <c r="I8" s="40">
+      <c r="I8" s="20">
         <v>1</v>
       </c>
-      <c r="J8" s="42">
+      <c r="J8" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:216" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="38" t="s">
+      <c r="D9" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="E9" s="59" t="s">
+      <c r="E9" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="F9" s="39">
+      <c r="F9" s="19">
         <v>43028</v>
       </c>
-      <c r="G9" s="40">
+      <c r="G9" s="20">
         <v>2</v>
       </c>
-      <c r="H9" s="39">
+      <c r="H9" s="19">
         <v>43029</v>
       </c>
-      <c r="I9" s="40">
+      <c r="I9" s="20">
         <v>2</v>
       </c>
-      <c r="J9" s="42">
+      <c r="J9" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:216" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="57" t="s">
+      <c r="B10" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="38" t="s">
+      <c r="D10" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="E10" s="59" t="s">
+      <c r="E10" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="F10" s="39">
+      <c r="F10" s="19">
         <v>43028</v>
       </c>
-      <c r="G10" s="40">
+      <c r="G10" s="20">
         <v>2</v>
       </c>
-      <c r="H10" s="39">
+      <c r="H10" s="19">
         <v>43029</v>
       </c>
-      <c r="I10" s="40">
+      <c r="I10" s="20">
         <v>2</v>
       </c>
-      <c r="J10" s="42">
+      <c r="J10" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:216" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="57" t="s">
+      <c r="B11" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="38" t="s">
+      <c r="C11" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="38" t="s">
+      <c r="D11" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="E11" s="59" t="s">
+      <c r="E11" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="39">
+      <c r="F11" s="19">
         <v>43028</v>
       </c>
-      <c r="G11" s="40">
+      <c r="G11" s="20">
         <v>2</v>
       </c>
-      <c r="H11" s="39">
+      <c r="H11" s="19">
         <v>43029</v>
       </c>
-      <c r="I11" s="40">
+      <c r="I11" s="20">
         <v>2</v>
       </c>
-      <c r="J11" s="42">
+      <c r="J11" s="22">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:216" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="37" t="s">
+      <c r="D12" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="60"/>
-      <c r="F12" s="39">
+      <c r="E12" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="19">
         <v>43033</v>
       </c>
-      <c r="G12" s="40">
+      <c r="G12" s="20">
         <v>2</v>
       </c>
-      <c r="H12" s="41"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="42">
+      <c r="H12" s="21"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:216" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="45" t="s">
+      <c r="B13" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="37" t="s">
+      <c r="C13" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="37" t="s">
+      <c r="D13" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="60"/>
-      <c r="F13" s="39">
+      <c r="E13" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="19">
         <f>G12+F12</f>
         <v>43035</v>
       </c>
-      <c r="G13" s="40">
+      <c r="G13" s="20">
         <v>5</v>
       </c>
-      <c r="H13" s="39"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="42">
+      <c r="H13" s="19"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:216" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="37" t="s">
+      <c r="C14" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="37" t="s">
+      <c r="D14" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="60"/>
-      <c r="F14" s="39">
+      <c r="E14" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="19">
         <f t="shared" ref="F14:F35" si="0">G13+F13</f>
         <v>43040</v>
       </c>
-      <c r="G14" s="40">
+      <c r="G14" s="20">
         <v>4</v>
       </c>
-      <c r="H14" s="39"/>
-      <c r="I14" s="40"/>
-      <c r="J14" s="42">
+      <c r="H14" s="19"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:216" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="45" t="s">
+      <c r="B15" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="37" t="s">
+      <c r="D15" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="60"/>
-      <c r="F15" s="39">
+      <c r="E15" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="19">
         <f t="shared" si="0"/>
         <v>43044</v>
       </c>
-      <c r="G15" s="40">
+      <c r="G15" s="20">
         <v>2</v>
       </c>
-      <c r="H15" s="39"/>
-      <c r="I15" s="40"/>
-      <c r="J15" s="42">
+      <c r="H15" s="19"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:216" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="37" t="s">
+      <c r="D16" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="60"/>
-      <c r="F16" s="39">
+      <c r="E16" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="19">
         <f t="shared" si="0"/>
         <v>43046</v>
       </c>
-      <c r="G16" s="40">
+      <c r="G16" s="20">
         <v>3</v>
       </c>
-      <c r="H16" s="39"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="42">
+      <c r="H16" s="19"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="37" t="s">
+      <c r="C17" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="37" t="s">
+      <c r="D17" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E17" s="60"/>
-      <c r="F17" s="39">
+      <c r="E17" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="19">
         <f t="shared" si="0"/>
         <v>43049</v>
       </c>
-      <c r="G17" s="40">
+      <c r="G17" s="20">
         <v>3</v>
       </c>
-      <c r="H17" s="39"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="42">
+      <c r="H17" s="19"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="45" t="s">
+      <c r="B18" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="37" t="s">
+      <c r="C18" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="37" t="s">
+      <c r="D18" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="60"/>
-      <c r="F18" s="39">
+      <c r="E18" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F18" s="19">
         <f t="shared" si="0"/>
         <v>43052</v>
       </c>
-      <c r="G18" s="40">
+      <c r="G18" s="20">
         <v>6</v>
       </c>
-      <c r="H18" s="39"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="42">
+      <c r="H18" s="19"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="45" t="s">
+      <c r="B19" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="37" t="s">
+      <c r="C19" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="37" t="s">
+      <c r="D19" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="60"/>
-      <c r="F19" s="39">
+      <c r="E19" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="19">
         <f t="shared" si="0"/>
         <v>43058</v>
       </c>
-      <c r="G19" s="40">
+      <c r="G19" s="20">
         <v>5</v>
       </c>
-      <c r="H19" s="39"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="42">
+      <c r="H19" s="19"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="45" t="s">
+      <c r="B20" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="37" t="s">
+      <c r="C20" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D20" s="37" t="s">
+      <c r="D20" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="60"/>
-      <c r="F20" s="39">
+      <c r="E20" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" s="19">
         <f t="shared" si="0"/>
         <v>43063</v>
       </c>
-      <c r="G20" s="40">
+      <c r="G20" s="20">
         <v>4</v>
       </c>
-      <c r="H20" s="39"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="42">
+      <c r="H20" s="19"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="45" t="s">
+      <c r="B21" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="37" t="s">
+      <c r="C21" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="37" t="s">
+      <c r="D21" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="60"/>
-      <c r="F21" s="39">
+      <c r="E21" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F21" s="19">
         <f t="shared" si="0"/>
         <v>43067</v>
       </c>
-      <c r="G21" s="40">
+      <c r="G21" s="20">
         <v>3</v>
       </c>
-      <c r="H21" s="39"/>
-      <c r="I21" s="40"/>
-      <c r="J21" s="42">
+      <c r="H21" s="19"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="45" t="s">
+      <c r="B22" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="37" t="s">
+      <c r="C22" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="37" t="s">
+      <c r="D22" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="E22" s="60"/>
-      <c r="F22" s="39">
+      <c r="E22" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" s="19">
         <f t="shared" si="0"/>
         <v>43070</v>
       </c>
-      <c r="G22" s="40">
+      <c r="G22" s="20">
         <v>3</v>
       </c>
-      <c r="H22" s="39"/>
-      <c r="I22" s="40"/>
-      <c r="J22" s="42">
+      <c r="H22" s="19"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="44" t="s">
+      <c r="B23" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="37" t="s">
+      <c r="C23" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="37" t="s">
+      <c r="D23" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E23" s="60"/>
-      <c r="F23" s="39">
+      <c r="E23" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="19">
         <v>43103</v>
       </c>
-      <c r="G23" s="40">
+      <c r="G23" s="20">
         <v>4</v>
       </c>
-      <c r="H23" s="39"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="42">
+      <c r="H23" s="19"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="44" t="s">
+      <c r="B24" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="37" t="s">
+      <c r="C24" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="37" t="s">
+      <c r="D24" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E24" s="60"/>
-      <c r="F24" s="39">
+      <c r="E24" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24" s="19">
         <f t="shared" si="0"/>
         <v>43107</v>
       </c>
-      <c r="G24" s="40">
+      <c r="G24" s="20">
         <v>7</v>
       </c>
-      <c r="H24" s="39"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="42">
+      <c r="H24" s="19"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="44" t="s">
+      <c r="B25" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="37" t="s">
+      <c r="C25" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="37" t="s">
+      <c r="D25" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="60"/>
-      <c r="F25" s="39">
+      <c r="E25" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="F25" s="19">
         <f t="shared" si="0"/>
         <v>43114</v>
       </c>
-      <c r="G25" s="40">
+      <c r="G25" s="20">
         <v>7</v>
       </c>
-      <c r="H25" s="39"/>
-      <c r="I25" s="40"/>
-      <c r="J25" s="42">
+      <c r="H25" s="19"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="44" t="s">
+      <c r="B26" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="37" t="s">
+      <c r="C26" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="37" t="s">
+      <c r="D26" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="E26" s="60"/>
-      <c r="F26" s="39">
+      <c r="E26" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="F26" s="19">
         <f t="shared" si="0"/>
         <v>43121</v>
       </c>
-      <c r="G26" s="40">
+      <c r="G26" s="20">
         <v>3</v>
       </c>
-      <c r="H26" s="39"/>
-      <c r="I26" s="40"/>
-      <c r="J26" s="42">
+      <c r="H26" s="19"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="44" t="s">
+      <c r="B27" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="37" t="s">
+      <c r="C27" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="37" t="s">
+      <c r="D27" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="E27" s="60"/>
-      <c r="F27" s="39">
+      <c r="E27" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F27" s="19">
         <f t="shared" si="0"/>
         <v>43124</v>
       </c>
-      <c r="G27" s="40">
+      <c r="G27" s="20">
         <v>3</v>
       </c>
-      <c r="H27" s="39"/>
-      <c r="I27" s="40"/>
-      <c r="J27" s="42">
+      <c r="H27" s="19"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="44" t="s">
+      <c r="B28" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="37" t="s">
+      <c r="C28" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D28" s="37" t="s">
+      <c r="D28" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E28" s="60"/>
-      <c r="F28" s="39">
+      <c r="E28" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="F28" s="19">
         <f t="shared" si="0"/>
         <v>43127</v>
       </c>
-      <c r="G28" s="40">
+      <c r="G28" s="20">
         <v>5</v>
       </c>
-      <c r="H28" s="39"/>
-      <c r="I28" s="40"/>
-      <c r="J28" s="42">
+      <c r="H28" s="19"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="43" t="s">
+      <c r="B29" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="37" t="s">
+      <c r="C29" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="37" t="s">
+      <c r="D29" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="60"/>
-      <c r="F29" s="39">
+      <c r="E29" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F29" s="19">
         <v>43146</v>
       </c>
-      <c r="G29" s="40">
+      <c r="G29" s="20">
         <v>5</v>
       </c>
-      <c r="H29" s="39"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="42">
+      <c r="H29" s="19"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="43" t="s">
+      <c r="B30" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="37" t="s">
+      <c r="C30" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="37" t="s">
+      <c r="D30" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="E30" s="60"/>
-      <c r="F30" s="39">
+      <c r="E30" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="F30" s="19">
         <f t="shared" si="0"/>
         <v>43151</v>
       </c>
-      <c r="G30" s="40">
+      <c r="G30" s="20">
         <v>7</v>
       </c>
-      <c r="H30" s="39"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="42">
+      <c r="H30" s="19"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="43" t="s">
+      <c r="B31" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="37" t="s">
+      <c r="C31" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D31" s="37" t="s">
+      <c r="D31" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="E31" s="60"/>
-      <c r="F31" s="39">
+      <c r="E31" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F31" s="19">
         <f t="shared" si="0"/>
         <v>43158</v>
       </c>
-      <c r="G31" s="40">
+      <c r="G31" s="20">
         <v>7</v>
       </c>
-      <c r="H31" s="39"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="42">
+      <c r="H31" s="19"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="43" t="s">
+      <c r="B32" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="37" t="s">
+      <c r="C32" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D32" s="37" t="s">
+      <c r="D32" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="E32" s="60"/>
-      <c r="F32" s="39">
+      <c r="E32" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="F32" s="19">
         <f t="shared" si="0"/>
         <v>43165</v>
       </c>
-      <c r="G32" s="40">
+      <c r="G32" s="20">
         <v>6</v>
       </c>
-      <c r="H32" s="39"/>
-      <c r="I32" s="40"/>
-      <c r="J32" s="42">
+      <c r="H32" s="19"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="43" t="s">
+      <c r="B33" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="37" t="s">
+      <c r="C33" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D33" s="37" t="s">
+      <c r="D33" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="E33" s="60"/>
-      <c r="F33" s="39">
+      <c r="E33" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="F33" s="19">
         <f t="shared" si="0"/>
         <v>43171</v>
       </c>
-      <c r="G33" s="40">
+      <c r="G33" s="20">
         <v>5</v>
       </c>
-      <c r="H33" s="39"/>
-      <c r="I33" s="40"/>
-      <c r="J33" s="42">
+      <c r="H33" s="19"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="34" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="46" t="s">
+      <c r="B34" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="38" t="s">
+      <c r="C34" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="38" t="s">
+      <c r="D34" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="E34" s="59"/>
-      <c r="F34" s="39">
+      <c r="E34" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="F34" s="19">
         <f t="shared" si="0"/>
         <v>43176</v>
       </c>
-      <c r="G34" s="40">
+      <c r="G34" s="20">
         <v>8</v>
       </c>
-      <c r="H34" s="39"/>
-      <c r="I34" s="40"/>
-      <c r="J34" s="42">
+      <c r="H34" s="19"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="43" t="s">
+      <c r="B35" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="38" t="s">
+      <c r="C35" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D35" s="38" t="s">
+      <c r="D35" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E35" s="59"/>
-      <c r="F35" s="39">
+      <c r="E35" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="F35" s="19">
         <f t="shared" si="0"/>
         <v>43184</v>
       </c>
-      <c r="G35" s="40">
+      <c r="G35" s="20">
         <v>8</v>
       </c>
-      <c r="H35" s="39"/>
-      <c r="I35" s="40"/>
-      <c r="J35" s="42">
+      <c r="H35" s="19"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="22">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
some shitty ex celular stuff
</commit_message>
<xml_diff>
--- a/reports/ProjectPlan.xlsx
+++ b/reports/ProjectPlan.xlsx
@@ -324,7 +324,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d;@"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -442,6 +442,13 @@
       <i/>
       <sz val="14"/>
       <color theme="7"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1" tint="0.24994659260841701"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -666,7 +673,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -849,6 +856,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1722,8 +1732,8 @@
   </sheetPr>
   <dimension ref="B1:HH35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2743,10 +2753,14 @@
       <c r="G12" s="20">
         <v>2</v>
       </c>
-      <c r="H12" s="21"/>
-      <c r="I12" s="20"/>
+      <c r="H12" s="61">
+        <v>43047</v>
+      </c>
+      <c r="I12" s="20">
+        <v>2</v>
+      </c>
       <c r="J12" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:216" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2769,10 +2783,14 @@
       <c r="G13" s="20">
         <v>5</v>
       </c>
-      <c r="H13" s="19"/>
-      <c r="I13" s="20"/>
+      <c r="H13" s="19">
+        <v>43053</v>
+      </c>
+      <c r="I13" s="20">
+        <v>5</v>
+      </c>
       <c r="J13" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:216" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2795,10 +2813,14 @@
       <c r="G14" s="20">
         <v>4</v>
       </c>
-      <c r="H14" s="19"/>
-      <c r="I14" s="20"/>
+      <c r="H14" s="19">
+        <v>43067</v>
+      </c>
+      <c r="I14" s="20">
+        <v>4</v>
+      </c>
       <c r="J14" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:216" ht="30" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>